<commit_message>
backend dev push 1
</commit_message>
<xml_diff>
--- a/noteshare_data_schema.xlsx
+++ b/noteshare_data_schema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/travisratnaharan/Documents/Work/noteshare/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{07079F7D-BD0B-4640-8E07-B77344698984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3821D46-8AD5-4B45-9FD6-E1367D5881AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41360" yWindow="500" windowWidth="28040" windowHeight="17440" activeTab="6" xr2:uid="{7B814040-DF51-274F-BB99-B8AE1F73AFA9}"/>
+    <workbookView xWindow="59300" yWindow="500" windowWidth="14940" windowHeight="17440" activeTab="2" xr2:uid="{7B814040-DF51-274F-BB99-B8AE1F73AFA9}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="15">
   <si>
     <t>id</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>public</t>
+  </si>
+  <si>
+    <t>page_count</t>
   </si>
 </sst>
 </file>
@@ -533,10 +536,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CDB81DA-D561-E14F-8A4B-5313B8A2A7F9}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -547,7 +550,7 @@
     <col min="7" max="7" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -567,10 +570,13 @@
         <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -581,7 +587,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -677,7 +683,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCD9EAAF-A267-6D4E-8B2B-05DAE4608BF0}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>

</xml_diff>